<commit_message>
Thêm mô tả trong thao tác thêm dữ liệu từ file + Thêm view khảo sát cho sinh viên
</commit_message>
<xml_diff>
--- a/static/web/excel/Data_KQHT_SV.xlsx
+++ b/static/web/excel/Data_KQHT_SV.xlsx
@@ -37,13 +37,13 @@
     <t>MSV</t>
   </si>
   <si>
+    <t>Phạm Hồng Nghĩa</t>
+  </si>
+  <si>
     <t>Dương Văn Nam</t>
   </si>
   <si>
     <t>Lã Đức Nam</t>
-  </si>
-  <si>
-    <t>Phạm Hồng Nghĩa</t>
   </si>
   <si>
     <t>K65A5</t>
@@ -445,7 +445,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>20002076</v>
+        <v>20002080</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -463,18 +463,18 @@
         <v>12</v>
       </c>
       <c r="G2">
-        <v>3.73</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>20002077</v>
+        <v>20002076</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>37588</v>
+        <v>37536</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -486,18 +486,18 @@
         <v>12</v>
       </c>
       <c r="G3">
-        <v>3.65</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>20002080</v>
+        <v>20002077</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>37536</v>
+        <v>37588</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -509,7 +509,7 @@
         <v>12</v>
       </c>
       <c r="G4">
-        <v>3.77</v>
+        <v>3.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>